<commit_message>
Update GSC export Excel files
Refreshed Breadcrumbs, Coverage, and Https Excel exports for heatlabs.net with latest data.
</commit_message>
<xml_diff>
--- a/gsc-export/heatlabs.net-Breadcrumbs.xlsx
+++ b/gsc-export/heatlabs.net-Breadcrumbs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>2025-11-01</t>
+  </si>
+  <si>
+    <t>2025-11-02</t>
   </si>
   <si>
     <t>Issue</t>
@@ -162,7 +165,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" rightToLeft="false"/>
   </sheetViews>
@@ -474,6 +477,17 @@
       </c>
       <c r="C28" t="n" s="0">
         <v>112.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C29" t="n" s="0">
+        <v>115.0</v>
       </c>
     </row>
   </sheetData>
@@ -491,13 +505,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -515,13 +529,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated GSC export Excel files
Refreshed Breadcrumbs, Coverage, Https, and Video-indexing Excel exports with new data for heatlabs.net.
</commit_message>
<xml_diff>
--- a/gsc-export/heatlabs.net-Breadcrumbs.xlsx
+++ b/gsc-export/heatlabs.net-Breadcrumbs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>2025-11-02</t>
+  </si>
+  <si>
+    <t>2025-11-03</t>
   </si>
   <si>
     <t>Issue</t>
@@ -165,7 +168,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" rightToLeft="false"/>
   </sheetViews>
@@ -488,6 +491,17 @@
       </c>
       <c r="C29" t="n" s="0">
         <v>115.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C30" t="n" s="0">
+        <v>108.0</v>
       </c>
     </row>
   </sheetData>
@@ -505,13 +519,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -529,13 +543,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated GSC export Excel files with latest data
</commit_message>
<xml_diff>
--- a/gsc-export/heatlabs.net-Breadcrumbs.xlsx
+++ b/gsc-export/heatlabs.net-Breadcrumbs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>2025-11-03</t>
+  </si>
+  <si>
+    <t>2025-11-04</t>
   </si>
   <si>
     <t>Issue</t>
@@ -168,7 +171,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" rightToLeft="false"/>
   </sheetViews>
@@ -502,6 +505,17 @@
       </c>
       <c r="C30" t="n" s="0">
         <v>108.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C31" t="n" s="0">
+        <v>105.0</v>
       </c>
     </row>
   </sheetData>
@@ -519,13 +533,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -543,13 +557,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>